<commit_message>
Remove duplicate County Connection line
</commit_message>
<xml_diff>
--- a/tm2py_utils/examples/temp_acceptance/canonical-agency-names.xlsx
+++ b/tm2py_utils/examples/temp_acceptance/canonical-agency-names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/tm2py/examples/temp_acceptance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tm2\tm2py-utils\tm2py_utils\examples\temp_acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5216FDEE-290A-004B-AFCF-280402575A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB518CD-574E-40DD-91D9-E3B42FD11688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="5900" windowWidth="37540" windowHeight="16940" xr2:uid="{13633017-C2A9-F34B-B7B9-245E0E090A18}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" xr2:uid="{13633017-C2A9-F34B-B7B9-245E0E090A18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>canonical_name</t>
   </si>
@@ -653,18 +653,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60A17E-6708-694D-9295-4A257F46B20A}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="40.83203125" customWidth="1"/>
+    <col min="1" max="6" width="40.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +684,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -695,7 +695,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -706,7 +706,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -714,7 +714,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -725,12 +725,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -741,7 +741,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -749,22 +749,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -772,234 +772,229 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
         <v>20</v>
       </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
         <v>24</v>
       </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
-    <sortCondition ref="A2:A41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C40">
+    <sortCondition ref="A2:A40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>